<commit_message>
Update data reading mechanism. Added functionality to import from xlsx.
git-svn-id: svn://biometris-nas.wurnet.nl/AMIGA@665 3ae013c2-4042-2242-b34d-985be216b4aa
</commit_message>
<xml_diff>
--- a/AmigaPowerAnalysis/AmigaPowerAnalysis.Tests/Resources/ExcelImportData1.xlsx
+++ b/AmigaPowerAnalysis/AmigaPowerAnalysis.Tests/Resources/ExcelImportData1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EndpointGroups" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>EndpointID</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Non-Target insects counts</t>
   </si>
   <si>
-    <t>Fraction</t>
-  </si>
-  <si>
     <t>PowerLaw</t>
   </si>
   <si>
@@ -111,6 +108,12 @@
   </si>
   <si>
     <t>NaN</t>
+  </si>
+  <si>
+    <t>Poisson</t>
+  </si>
+  <si>
+    <t>OverdispersedPoisson</t>
   </si>
 </sst>
 </file>
@@ -451,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +472,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -490,18 +493,18 @@
         <v>7</v>
       </c>
       <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
         <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>0.5</v>
@@ -510,7 +513,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -527,10 +530,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>0.5</v>
@@ -539,7 +542,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -556,10 +559,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
       </c>
       <c r="C4">
         <v>0.5</v>
@@ -568,7 +571,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -585,19 +588,19 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>0.95</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -617,7 +620,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>0.5</v>
@@ -626,7 +629,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -648,10 +651,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,15 +664,14 @@
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -689,25 +691,22 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -715,7 +714,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>0.02</v>
@@ -724,36 +723,33 @@
         <v>0.999</v>
       </c>
       <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>90</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>15</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0.5</v>
-      </c>
-      <c r="J2">
-        <v>90</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>0.05</v>
@@ -762,36 +758,33 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>18</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>100</v>
-      </c>
-      <c r="K3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>0.02</v>
@@ -800,36 +793,33 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="H4">
-        <v>1.7</v>
+        <v>10</v>
       </c>
       <c r="I4">
-        <v>10</v>
-      </c>
-      <c r="J4">
         <v>100</v>
       </c>
-      <c r="K4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>0.02</v>
@@ -838,36 +828,33 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="H5">
-        <v>1.7</v>
+        <v>10</v>
       </c>
       <c r="I5">
-        <v>10</v>
-      </c>
-      <c r="J5">
         <v>100</v>
       </c>
-      <c r="K5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>0.01</v>
@@ -876,24 +863,21 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="H6">
-        <v>1.7</v>
+        <v>10</v>
       </c>
       <c r="I6">
-        <v>10</v>
-      </c>
-      <c r="J6">
         <v>100</v>
       </c>
-      <c r="K6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6">
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <v>0</v>
       </c>
     </row>

</xml_diff>